<commit_message>
Example Push Git Hub
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peerschwertfeger/Documents/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/Fitbit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3C42D3-7C46-104D-BB42-25308BAA2EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BB79D6-F0E9-7C43-B1B4-2BE45ED7179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{4F0FB0B0-39D8-154D-B13B-3B537C5CF837}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,6 +542,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
+      <c r="F5">
+        <v>34628</v>
+      </c>
       <c r="I5" s="4">
         <v>44413</v>
       </c>

</xml_diff>

<commit_message>
update SJT r script
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/Fitbit/Heart Rate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\Fitbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peerschwertfeger/Documents/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/Fitbit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{9FE82235-59EC-4842-BC6E-912145EDE606}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53BD06F-DDF8-FA44-97F5-CA42DABA7117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="16236" xr2:uid="{4F0FB0B0-39D8-154D-B13B-3B537C5CF837}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{4F0FB0B0-39D8-154D-B13B-3B537C5CF837}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID participant</t>
   </si>
@@ -58,9 +67,6 @@
   </si>
   <si>
     <t>Missing</t>
-  </si>
-  <si>
-    <t>19.01.20021</t>
   </si>
 </sst>
 </file>
@@ -226,6 +232,14 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
@@ -257,7 +271,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -297,14 +311,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -364,14 +378,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -391,7 +405,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -431,14 +445,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -458,7 +472,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -498,14 +512,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -525,7 +539,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -565,14 +579,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -592,7 +606,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -632,14 +646,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -659,7 +673,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -699,14 +713,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -726,7 +740,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -766,14 +780,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -793,7 +807,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -833,14 +847,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -860,7 +874,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -900,14 +914,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -927,7 +941,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -967,14 +981,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -994,7 +1008,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1034,14 +1048,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1061,7 +1075,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1101,14 +1115,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1128,7 +1142,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1168,14 +1182,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1195,7 +1209,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1235,14 +1249,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1262,7 +1276,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1302,14 +1316,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1329,7 +1343,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1369,14 +1383,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1396,7 +1410,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1436,14 +1450,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1463,7 +1477,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1503,14 +1517,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1530,7 +1544,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1570,14 +1584,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1597,7 +1611,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1637,14 +1651,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1664,7 +1678,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1704,14 +1718,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1731,7 +1745,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1771,14 +1785,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1798,7 +1812,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1838,14 +1852,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1865,7 +1879,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1905,14 +1919,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1932,7 +1946,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -1972,14 +1986,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -1999,7 +2013,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -2039,14 +2053,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -2066,7 +2080,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -2106,14 +2120,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -2133,7 +2147,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>15240</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
@@ -2151,7 +2165,7 @@
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5125200C-B4DD-4D85-A6D2-885C930DE46B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2173,14 +2187,14 @@
               <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
                 <a14:hiddenFill>
                   <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a14:hiddenFill>
               </a:ext>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
@@ -2192,6 +2206,135 @@
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1057" name="Check Box 33" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="1225550" cy="206375"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1058" name="Check Box 34" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{050925E5-C2BB-964E-96C5-2BE88D92B451}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2501,20 +2644,20 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.69921875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.296875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="20.69921875" customWidth="1"/>
-    <col min="7" max="7" width="17.796875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.796875" customWidth="1"/>
-    <col min="10" max="10" width="16.19921875" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101</v>
       </c>
@@ -2578,7 +2721,7 @@
         <v>44398</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>102</v>
       </c>
@@ -2607,7 +2750,7 @@
         <v>44404</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>103</v>
       </c>
@@ -2630,7 +2773,7 @@
         <v>44405</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>104</v>
       </c>
@@ -2659,7 +2802,7 @@
         <v>44413</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>201</v>
       </c>
@@ -2688,7 +2831,7 @@
         <v>44439</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>105</v>
       </c>
@@ -2717,7 +2860,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>106</v>
       </c>
@@ -2746,7 +2889,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>202</v>
       </c>
@@ -2775,7 +2918,7 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>203</v>
       </c>
@@ -2804,7 +2947,7 @@
         <v>44474</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>107</v>
       </c>
@@ -2833,7 +2976,7 @@
         <v>44475</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>108</v>
       </c>
@@ -2863,7 +3006,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>109</v>
       </c>
@@ -2893,7 +3036,7 @@
         <v>44487</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>110</v>
       </c>
@@ -2922,7 +3065,7 @@
         <v>44508</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>111</v>
       </c>
@@ -2952,7 +3095,7 @@
         <v>44515</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>112</v>
       </c>
@@ -2982,7 +3125,7 @@
         <v>44547</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>205</v>
       </c>
@@ -3012,7 +3155,7 @@
         <v>44526</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>206</v>
       </c>
@@ -3041,7 +3184,7 @@
         <v>44568</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>113</v>
       </c>
@@ -3071,7 +3214,7 @@
         <v>44571</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>207</v>
       </c>
@@ -3101,7 +3244,7 @@
         <v>44578</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>114</v>
       </c>
@@ -3131,7 +3274,7 @@
         <v>44572</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>115</v>
       </c>
@@ -3157,29 +3300,71 @@
         <f>G22-F22</f>
         <v>567</v>
       </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I22" s="4">
+        <v>44580</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>116</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.57708333333333328</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="F23" s="6">
+        <v>170</v>
+      </c>
+      <c r="G23" s="6">
+        <v>630</v>
+      </c>
+      <c r="H23" s="6">
+        <f>G23-F23</f>
+        <v>460</v>
+      </c>
+      <c r="I23" s="4">
+        <v>44585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>117</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.56736111111111109</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="F24" s="6">
+        <v>38</v>
+      </c>
+      <c r="G24" s="6">
+        <v>38</v>
+      </c>
+      <c r="H24" s="6">
+        <f>G24-F24</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3188,7 +3373,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3197,7 +3382,7 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3206,7 +3391,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3215,7 +3400,7 @@
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3224,7 +3409,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3233,7 +3418,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3242,7 +3427,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3251,7 +3436,7 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3260,7 +3445,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -3269,7 +3454,7 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3278,7 +3463,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3287,7 +3472,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3296,7 +3481,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3305,7 +3490,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3314,7 +3499,7 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3323,7 +3508,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3332,492 +3517,492 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
     </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
       <c r="H74" s="6"/>
     </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
     </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
     </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
     </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
     </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
     </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
     </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
     </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
     </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
     </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
     </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
       <c r="H94" s="6"/>
     </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
     </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
       <c r="H96" s="6"/>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
       <c r="H97" s="6"/>
     </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
       <c r="H98" s="6"/>
     </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="6"/>
     </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
       <c r="H100" s="6"/>
     </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
       <c r="H101" s="6"/>
     </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
     </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
     </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
       <c r="H104" s="6"/>
     </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
     </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
       <c r="H106" s="6"/>
     </row>
-    <row r="107" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
       <c r="H107" s="6"/>
     </row>
-    <row r="108" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
       <c r="H108" s="6"/>
     </row>
-    <row r="109" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
       <c r="H109" s="6"/>
     </row>
-    <row r="110" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
       <c r="H110" s="6"/>
     </row>
-    <row r="111" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
       <c r="H111" s="6"/>
     </row>
-    <row r="112" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
     </row>
-    <row r="113" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
     </row>
-    <row r="114" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
       <c r="H114" s="6"/>
     </row>
-    <row r="115" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
       <c r="H115" s="6"/>
     </row>
-    <row r="116" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
       <c r="H116" s="6"/>
     </row>
-    <row r="117" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
       <c r="H117" s="6"/>
     </row>
-    <row r="118" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
     </row>
-    <row r="119" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
       <c r="H119" s="6"/>
     </row>
-    <row r="120" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
     </row>
-    <row r="121" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
       <c r="H121" s="6"/>
     </row>
-    <row r="122" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
-    <row r="123" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
       <c r="H123" s="6"/>
     </row>
-    <row r="124" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
       <c r="H124" s="6"/>
     </row>
-    <row r="125" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
       <c r="H125" s="6"/>
     </row>
-    <row r="126" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
     </row>
-    <row r="127" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
       <c r="H127" s="6"/>
     </row>
-    <row r="128" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
       <c r="H128" s="6"/>
     </row>
-    <row r="129" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
       <c r="H129" s="6"/>
     </row>
-    <row r="130" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
       <c r="H130" s="6"/>
     </row>
-    <row r="131" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
       <c r="H131" s="6"/>
     </row>
-    <row r="132" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
       <c r="H132" s="6"/>
     </row>
-    <row r="133" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
       <c r="H133" s="6"/>
     </row>
-    <row r="134" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F134" s="6"/>
       <c r="G134" s="6"/>
       <c r="H134" s="6"/>
     </row>
-    <row r="135" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
       <c r="H135" s="6"/>
     </row>
-    <row r="136" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F136" s="6"/>
       <c r="G136" s="6"/>
       <c r="H136" s="6"/>
     </row>
-    <row r="137" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
       <c r="H137" s="6"/>
     </row>
-    <row r="138" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F138" s="6"/>
       <c r="G138" s="6"/>
       <c r="H138" s="6"/>
     </row>
-    <row r="139" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F139" s="6"/>
       <c r="G139" s="6"/>
       <c r="H139" s="6"/>
@@ -3837,7 +4022,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3881,7 +4066,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3903,7 +4088,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3925,7 +4110,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3947,7 +4132,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3969,7 +4154,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -3991,7 +4176,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4013,7 +4198,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4035,7 +4220,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4057,7 +4242,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4079,7 +4264,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4101,7 +4286,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4123,7 +4308,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4145,7 +4330,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4167,7 +4352,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4189,7 +4374,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4211,7 +4396,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4233,7 +4418,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4255,7 +4440,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>12</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4277,7 +4462,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4299,7 +4484,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4321,7 +4506,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4343,7 +4528,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>16</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4365,7 +4550,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>17</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4387,7 +4572,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4409,7 +4594,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4431,7 +4616,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4453,7 +4638,7 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>15240</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>21</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
@@ -4461,6 +4646,50 @@
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>22</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1057" r:id="rId33" name="Check Box 33">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1058" r:id="rId34" name="Check Box 34">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>9</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>23</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>